<commit_message>
upd 29 apr v2
</commit_message>
<xml_diff>
--- a/useful/time_sheet.xlsx
+++ b/useful/time_sheet.xlsx
@@ -281,7 +281,7 @@
     <t>= recurent</t>
   </si>
   <si>
-    <t>Create functional links to proper pages in header menu</t>
+    <t>Create functional links to proper pages on site, in header menu</t>
   </si>
 </sst>
 </file>
@@ -679,6 +679,51 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -694,56 +739,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:HT101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1070,55 +1070,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:228" x14ac:dyDescent="0.25">
-      <c r="B1" s="64"/>
-      <c r="C1" s="69" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="G1" s="62" t="s">
+      <c r="D1" s="55"/>
+      <c r="G1" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
       <c r="J1" s="23"/>
       <c r="K1" s="24"/>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
       <c r="Q1" s="20"/>
       <c r="R1" s="25"/>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
       <c r="X1" s="20"/>
       <c r="Y1" s="26"/>
-      <c r="Z1" s="51" t="s">
+      <c r="Z1" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="52"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="67"/>
       <c r="AF1" s="21"/>
       <c r="AG1" s="21"/>
       <c r="AH1" s="22"/>
       <c r="AI1" s="22"/>
     </row>
     <row r="2" spans="1:228" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="68" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="68"/>
+      <c r="D2" s="59"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
@@ -1150,11 +1150,11 @@
       <c r="AI2" s="22"/>
     </row>
     <row r="3" spans="1:228" x14ac:dyDescent="0.25">
-      <c r="B3" s="67"/>
-      <c r="C3" s="68" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="12"/>
       <c r="G3" s="15" t="s">
         <v>13</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="F4" s="42">
         <f t="shared" ref="F4:BQ4" si="0">SUM(F6:F101)</f>
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G4" s="47">
         <f t="shared" si="0"/>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="J4" s="48">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K4" s="49">
         <f t="shared" si="0"/>
@@ -3400,13 +3400,13 @@
       </c>
     </row>
     <row r="6" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="57" t="s">
+      <c r="B6" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="52">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="12" t="s">
@@ -3490,9 +3490,9 @@
       <c r="HS6" s="7"/>
     </row>
     <row r="7" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="65">
+      <c r="B7" s="64"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="52">
         <v>1.2</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -3578,9 +3578,9 @@
       <c r="HS7" s="7"/>
     </row>
     <row r="8" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="65">
+      <c r="B8" s="64"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="52">
         <v>1.3</v>
       </c>
       <c r="E8" s="12" t="s">
@@ -3664,8 +3664,8 @@
       <c r="HS8" s="7"/>
     </row>
     <row r="9" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="60"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="38">
         <v>1.4</v>
       </c>
@@ -3749,8 +3749,8 @@
       <c r="HS9" s="7"/>
     </row>
     <row r="10" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="57"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="38">
         <v>1.5</v>
       </c>
@@ -3832,9 +3832,9 @@
       <c r="HS10" s="7"/>
     </row>
     <row r="11" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="71">
+      <c r="B11" s="64"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="57">
         <v>1.6</v>
       </c>
       <c r="E11" s="12" t="s">
@@ -3842,10 +3842,12 @@
       </c>
       <c r="F11" s="45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7">
+        <v>1</v>
+      </c>
       <c r="L11" s="9"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -3915,8 +3917,8 @@
       <c r="HS11" s="7"/>
     </row>
     <row r="12" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="60"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="38">
         <v>1.7</v>
       </c>
@@ -3998,9 +4000,9 @@
       <c r="HS12" s="7"/>
     </row>
     <row r="13" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="65">
+      <c r="B13" s="64"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="52">
         <v>1.8</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -4084,9 +4086,9 @@
       <c r="HS13" s="7"/>
     </row>
     <row r="14" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="71">
+      <c r="B14" s="64"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="57">
         <v>1.9</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -4094,10 +4096,12 @@
       </c>
       <c r="F14" s="45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7">
+        <v>6</v>
+      </c>
       <c r="L14" s="9"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
@@ -4167,9 +4171,9 @@
       <c r="HS14" s="7"/>
     </row>
     <row r="15" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="72">
+      <c r="B15" s="64"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="58">
         <v>1.1000000000000001</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -4252,8 +4256,8 @@
       <c r="HS15" s="7"/>
     </row>
     <row r="16" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="61"/>
-      <c r="C16" s="58"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="37"/>
       <c r="E16" s="14" t="s">
         <v>44</v>
@@ -4333,13 +4337,13 @@
       <c r="HS16" s="7"/>
     </row>
     <row r="17" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="66">
+      <c r="D17" s="53">
         <v>2.1</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -4422,8 +4426,8 @@
       <c r="HS17" s="7"/>
     </row>
     <row r="18" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="38">
         <v>2.2000000000000002</v>
       </c>
@@ -4505,8 +4509,8 @@
       <c r="HS18" s="7"/>
     </row>
     <row r="19" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="60"/>
-      <c r="C19" s="57"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="38">
         <v>2.2999999999999998</v>
       </c>
@@ -4588,9 +4592,9 @@
       <c r="HS19" s="7"/>
     </row>
     <row r="20" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="60"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="65">
+      <c r="B20" s="64"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="52">
         <v>2.4</v>
       </c>
       <c r="E20" s="12" t="s">
@@ -4673,8 +4677,8 @@
       <c r="HS20" s="7"/>
     </row>
     <row r="21" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="57"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="38">
         <v>2.5</v>
       </c>
@@ -4683,10 +4687,12 @@
       </c>
       <c r="F21" s="45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="7">
+        <v>2</v>
+      </c>
       <c r="L21" s="9"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
@@ -4756,8 +4762,8 @@
       <c r="HS21" s="7"/>
     </row>
     <row r="22" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="60"/>
-      <c r="C22" s="57"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="38">
         <v>2.6</v>
       </c>
@@ -4837,8 +4843,8 @@
       <c r="HS22" s="7"/>
     </row>
     <row r="23" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="60"/>
-      <c r="C23" s="57"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="38">
         <v>2.7</v>
       </c>
@@ -4918,8 +4924,8 @@
       <c r="HS23" s="7"/>
     </row>
     <row r="24" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="60"/>
-      <c r="C24" s="57"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="38">
         <v>2.8</v>
       </c>
@@ -4999,8 +5005,8 @@
       <c r="HS24" s="7"/>
     </row>
     <row r="25" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="57"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="38">
         <v>2.9</v>
       </c>
@@ -5080,8 +5086,8 @@
       <c r="HS25" s="7"/>
     </row>
     <row r="26" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="61"/>
-      <c r="C26" s="58"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="37"/>
       <c r="E26" s="14" t="s">
         <v>44</v>
@@ -5161,10 +5167,10 @@
       <c r="HS26" s="7"/>
     </row>
     <row r="27" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="62" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="39">
@@ -5248,8 +5254,8 @@
       <c r="HS27" s="7"/>
     </row>
     <row r="28" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="60"/>
-      <c r="C28" s="57"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="38">
         <v>3.2</v>
       </c>
@@ -5331,8 +5337,8 @@
       <c r="HS28" s="7"/>
     </row>
     <row r="29" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="60"/>
-      <c r="C29" s="57"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="60"/>
       <c r="D29" s="38">
         <v>3.3</v>
       </c>
@@ -5414,8 +5420,8 @@
       <c r="HS29" s="7"/>
     </row>
     <row r="30" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="60"/>
-      <c r="C30" s="57"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="38">
         <v>3.4</v>
       </c>
@@ -5497,8 +5503,8 @@
       <c r="HS30" s="7"/>
     </row>
     <row r="31" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="60"/>
-      <c r="C31" s="57"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="60"/>
       <c r="D31" s="38">
         <v>3.5</v>
       </c>
@@ -5580,8 +5586,8 @@
       <c r="HS31" s="7"/>
     </row>
     <row r="32" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="60"/>
-      <c r="C32" s="57"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="38">
         <v>3.6</v>
       </c>
@@ -5663,8 +5669,8 @@
       <c r="HS32" s="7"/>
     </row>
     <row r="33" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="60"/>
-      <c r="C33" s="57"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="38">
         <v>3.7</v>
       </c>
@@ -5746,8 +5752,8 @@
       <c r="HS33" s="7"/>
     </row>
     <row r="34" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="60"/>
-      <c r="C34" s="57"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="38">
         <v>3.8</v>
       </c>
@@ -5829,8 +5835,8 @@
       <c r="HS34" s="7"/>
     </row>
     <row r="35" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="60"/>
-      <c r="C35" s="57"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="38">
         <v>3.9</v>
       </c>
@@ -5910,8 +5916,8 @@
       <c r="HS35" s="7"/>
     </row>
     <row r="36" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="61"/>
-      <c r="C36" s="58"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="37"/>
       <c r="E36" s="14" t="s">
         <v>44</v>
@@ -5991,10 +5997,10 @@
       <c r="HS36" s="7"/>
     </row>
     <row r="37" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="62" t="s">
         <v>21</v>
       </c>
       <c r="D37" s="39">
@@ -6078,8 +6084,8 @@
       <c r="HS37" s="7"/>
     </row>
     <row r="38" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="60"/>
-      <c r="C38" s="57"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="38">
         <v>4.2</v>
       </c>
@@ -6161,8 +6167,8 @@
       <c r="HS38" s="7"/>
     </row>
     <row r="39" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="60"/>
-      <c r="C39" s="57"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="38">
         <v>4.3</v>
       </c>
@@ -6244,8 +6250,8 @@
       <c r="HS39" s="7"/>
     </row>
     <row r="40" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="60"/>
-      <c r="C40" s="57"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="38">
         <v>4.4000000000000004</v>
       </c>
@@ -6327,8 +6333,8 @@
       <c r="HS40" s="7"/>
     </row>
     <row r="41" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="60"/>
-      <c r="C41" s="57"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="60"/>
       <c r="D41" s="38">
         <v>4.5</v>
       </c>
@@ -6410,8 +6416,8 @@
       <c r="HS41" s="7"/>
     </row>
     <row r="42" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="60"/>
-      <c r="C42" s="57"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="60"/>
       <c r="D42" s="38">
         <v>4.5999999999999996</v>
       </c>
@@ -6493,8 +6499,8 @@
       <c r="HS42" s="7"/>
     </row>
     <row r="43" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="60"/>
-      <c r="C43" s="57"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="38">
         <v>4.7</v>
       </c>
@@ -6576,8 +6582,8 @@
       <c r="HS43" s="7"/>
     </row>
     <row r="44" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="60"/>
-      <c r="C44" s="57"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="60"/>
       <c r="D44" s="38">
         <v>4.8</v>
       </c>
@@ -6659,8 +6665,8 @@
       <c r="HS44" s="7"/>
     </row>
     <row r="45" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="60"/>
-      <c r="C45" s="57"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="60"/>
       <c r="D45" s="38">
         <v>4.9000000000000004</v>
       </c>
@@ -6740,8 +6746,8 @@
       <c r="HS45" s="7"/>
     </row>
     <row r="46" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="60"/>
-      <c r="C46" s="57"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="60"/>
       <c r="D46" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -6821,8 +6827,8 @@
       <c r="HS46" s="7"/>
     </row>
     <row r="47" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="61"/>
-      <c r="C47" s="58"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="61"/>
       <c r="D47" s="37"/>
       <c r="E47" s="14" t="s">
         <v>44</v>
@@ -6902,10 +6908,10 @@
       <c r="HS47" s="7"/>
     </row>
     <row r="48" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="56" t="s">
+      <c r="C48" s="62" t="s">
         <v>30</v>
       </c>
       <c r="D48" s="39">
@@ -6989,8 +6995,8 @@
       <c r="HS48" s="7"/>
     </row>
     <row r="49" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="60"/>
-      <c r="C49" s="57"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="60"/>
       <c r="D49" s="38">
         <v>5.2</v>
       </c>
@@ -7072,8 +7078,8 @@
       <c r="HS49" s="7"/>
     </row>
     <row r="50" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="60"/>
-      <c r="C50" s="57"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="60"/>
       <c r="D50" s="38">
         <v>5.3</v>
       </c>
@@ -7155,8 +7161,8 @@
       <c r="HS50" s="7"/>
     </row>
     <row r="51" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="60"/>
-      <c r="C51" s="57"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="60"/>
       <c r="D51" s="38">
         <v>5.4</v>
       </c>
@@ -7238,8 +7244,8 @@
       <c r="HS51" s="7"/>
     </row>
     <row r="52" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="60"/>
-      <c r="C52" s="57"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="60"/>
       <c r="D52" s="38">
         <v>5.5</v>
       </c>
@@ -7321,8 +7327,8 @@
       <c r="HS52" s="7"/>
     </row>
     <row r="53" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="60"/>
-      <c r="C53" s="57"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="60"/>
       <c r="D53" s="38">
         <v>5.6</v>
       </c>
@@ -7404,8 +7410,8 @@
       <c r="HS53" s="7"/>
     </row>
     <row r="54" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="60"/>
-      <c r="C54" s="57"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="60"/>
       <c r="D54" s="38">
         <v>5.7</v>
       </c>
@@ -7487,8 +7493,8 @@
       <c r="HS54" s="7"/>
     </row>
     <row r="55" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="60"/>
-      <c r="C55" s="57"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="60"/>
       <c r="D55" s="38">
         <v>5.8</v>
       </c>
@@ -7568,8 +7574,8 @@
       <c r="HS55" s="7"/>
     </row>
     <row r="56" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="60"/>
-      <c r="C56" s="57"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="60"/>
       <c r="D56" s="38">
         <v>5.9</v>
       </c>
@@ -7649,8 +7655,8 @@
       <c r="HS56" s="7"/>
     </row>
     <row r="57" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="61"/>
-      <c r="C57" s="58"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="61"/>
       <c r="D57" s="37"/>
       <c r="E57" s="14" t="s">
         <v>44</v>
@@ -7730,10 +7736,10 @@
       <c r="HS57" s="7"/>
     </row>
     <row r="58" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="59" t="s">
+      <c r="B58" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="62" t="s">
         <v>69</v>
       </c>
       <c r="D58" s="39">
@@ -7817,8 +7823,8 @@
       <c r="HS58" s="7"/>
     </row>
     <row r="59" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="60"/>
-      <c r="C59" s="57"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="60"/>
       <c r="D59" s="38">
         <v>6.2</v>
       </c>
@@ -7900,8 +7906,8 @@
       <c r="HS59" s="7"/>
     </row>
     <row r="60" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="60"/>
-      <c r="C60" s="57"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="60"/>
       <c r="D60" s="38">
         <v>6.3</v>
       </c>
@@ -7981,8 +7987,8 @@
       <c r="HS60" s="7"/>
     </row>
     <row r="61" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="60"/>
-      <c r="C61" s="57"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="60"/>
       <c r="D61" s="38">
         <v>6.4</v>
       </c>
@@ -8062,8 +8068,8 @@
       <c r="HS61" s="7"/>
     </row>
     <row r="62" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="60"/>
-      <c r="C62" s="57"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="60"/>
       <c r="D62" s="38">
         <v>6.5</v>
       </c>
@@ -8143,8 +8149,8 @@
       <c r="HS62" s="7"/>
     </row>
     <row r="63" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B63" s="60"/>
-      <c r="C63" s="57"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="60"/>
       <c r="D63" s="38">
         <v>6.6</v>
       </c>
@@ -8224,8 +8230,8 @@
       <c r="HS63" s="7"/>
     </row>
     <row r="64" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="60"/>
-      <c r="C64" s="57"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="60"/>
       <c r="D64" s="38">
         <v>6.7</v>
       </c>
@@ -8305,8 +8311,8 @@
       <c r="HS64" s="7"/>
     </row>
     <row r="65" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="60"/>
-      <c r="C65" s="57"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="60"/>
       <c r="D65" s="38">
         <v>6.8</v>
       </c>
@@ -8386,8 +8392,8 @@
       <c r="HS65" s="7"/>
     </row>
     <row r="66" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="60"/>
-      <c r="C66" s="57"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="60"/>
       <c r="D66" s="38">
         <v>6.9</v>
       </c>
@@ -8467,8 +8473,8 @@
       <c r="HS66" s="7"/>
     </row>
     <row r="67" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="61"/>
-      <c r="C67" s="58"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="61"/>
       <c r="D67" s="37"/>
       <c r="E67" s="14" t="s">
         <v>44</v>
@@ -8548,10 +8554,10 @@
       <c r="HS67" s="7"/>
     </row>
     <row r="68" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="59" t="s">
+      <c r="B68" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="62" t="s">
         <v>66</v>
       </c>
       <c r="D68" s="39">
@@ -8635,8 +8641,8 @@
       <c r="HS68" s="7"/>
     </row>
     <row r="69" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="60"/>
-      <c r="C69" s="57"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="60"/>
       <c r="D69" s="38">
         <v>7.2</v>
       </c>
@@ -8718,8 +8724,8 @@
       <c r="HS69" s="7"/>
     </row>
     <row r="70" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="60"/>
-      <c r="C70" s="57"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="60"/>
       <c r="D70" s="38">
         <v>7.3</v>
       </c>
@@ -8801,8 +8807,8 @@
       <c r="HS70" s="7"/>
     </row>
     <row r="71" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="60"/>
-      <c r="C71" s="57"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="60"/>
       <c r="D71" s="38">
         <v>7.4</v>
       </c>
@@ -8884,8 +8890,8 @@
       <c r="HS71" s="7"/>
     </row>
     <row r="72" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="60"/>
-      <c r="C72" s="57"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="60"/>
       <c r="D72" s="38">
         <v>7.5</v>
       </c>
@@ -8967,8 +8973,8 @@
       <c r="HS72" s="7"/>
     </row>
     <row r="73" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="60"/>
-      <c r="C73" s="57"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="60"/>
       <c r="D73" s="38">
         <v>7.6</v>
       </c>
@@ -9048,8 +9054,8 @@
       <c r="HS73" s="7"/>
     </row>
     <row r="74" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B74" s="60"/>
-      <c r="C74" s="57"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="60"/>
       <c r="D74" s="38">
         <v>7.7</v>
       </c>
@@ -9129,8 +9135,8 @@
       <c r="HS74" s="7"/>
     </row>
     <row r="75" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="60"/>
-      <c r="C75" s="57"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="60"/>
       <c r="D75" s="38">
         <v>7.8</v>
       </c>
@@ -9210,8 +9216,8 @@
       <c r="HS75" s="7"/>
     </row>
     <row r="76" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B76" s="60"/>
-      <c r="C76" s="57"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="60"/>
       <c r="D76" s="38">
         <v>7.9</v>
       </c>
@@ -9291,8 +9297,8 @@
       <c r="HS76" s="7"/>
     </row>
     <row r="77" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B77" s="61"/>
-      <c r="C77" s="58"/>
+      <c r="B77" s="65"/>
+      <c r="C77" s="61"/>
       <c r="D77" s="37"/>
       <c r="E77" s="14" t="s">
         <v>44</v>
@@ -9372,10 +9378,10 @@
       <c r="HS77" s="7"/>
     </row>
     <row r="78" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="53" t="s">
+      <c r="B78" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="56" t="s">
+      <c r="C78" s="62" t="s">
         <v>55</v>
       </c>
       <c r="D78" s="39">
@@ -9457,8 +9463,8 @@
       <c r="HS78" s="7"/>
     </row>
     <row r="79" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="54"/>
-      <c r="C79" s="57"/>
+      <c r="B79" s="69"/>
+      <c r="C79" s="60"/>
       <c r="D79" s="38">
         <v>7.2</v>
       </c>
@@ -9538,8 +9544,8 @@
       <c r="HS79" s="7"/>
     </row>
     <row r="80" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="54"/>
-      <c r="C80" s="57"/>
+      <c r="B80" s="69"/>
+      <c r="C80" s="60"/>
       <c r="D80" s="38">
         <v>7.3</v>
       </c>
@@ -9619,8 +9625,8 @@
       <c r="HS80" s="7"/>
     </row>
     <row r="81" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="54"/>
-      <c r="C81" s="57"/>
+      <c r="B81" s="69"/>
+      <c r="C81" s="60"/>
       <c r="D81" s="38">
         <v>7.4</v>
       </c>
@@ -9700,8 +9706,8 @@
       <c r="HS81" s="7"/>
     </row>
     <row r="82" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="54"/>
-      <c r="C82" s="57"/>
+      <c r="B82" s="69"/>
+      <c r="C82" s="60"/>
       <c r="D82" s="38">
         <v>7.5</v>
       </c>
@@ -9781,8 +9787,8 @@
       <c r="HS82" s="7"/>
     </row>
     <row r="83" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="54"/>
-      <c r="C83" s="57"/>
+      <c r="B83" s="69"/>
+      <c r="C83" s="60"/>
       <c r="D83" s="38">
         <v>7.6</v>
       </c>
@@ -9862,8 +9868,8 @@
       <c r="HS83" s="7"/>
     </row>
     <row r="84" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="54"/>
-      <c r="C84" s="57"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="60"/>
       <c r="D84" s="38">
         <v>7.7</v>
       </c>
@@ -9943,8 +9949,8 @@
       <c r="HS84" s="7"/>
     </row>
     <row r="85" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="54"/>
-      <c r="C85" s="57"/>
+      <c r="B85" s="69"/>
+      <c r="C85" s="60"/>
       <c r="D85" s="38">
         <v>7.8</v>
       </c>
@@ -10024,8 +10030,8 @@
       <c r="HS85" s="7"/>
     </row>
     <row r="86" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="54"/>
-      <c r="C86" s="57"/>
+      <c r="B86" s="69"/>
+      <c r="C86" s="60"/>
       <c r="D86" s="38">
         <v>7.9</v>
       </c>
@@ -10105,8 +10111,8 @@
       <c r="HS86" s="7"/>
     </row>
     <row r="87" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="55"/>
-      <c r="C87" s="58"/>
+      <c r="B87" s="70"/>
+      <c r="C87" s="61"/>
       <c r="D87" s="37"/>
       <c r="E87" s="14" t="s">
         <v>44</v>
@@ -11251,11 +11257,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C6:C16"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="B17:B26"/>
-    <mergeCell ref="C27:C36"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="Z1:AE1"/>
     <mergeCell ref="S1:W1"/>
@@ -11272,6 +11273,11 @@
     <mergeCell ref="B37:B47"/>
     <mergeCell ref="B48:B57"/>
     <mergeCell ref="C48:C57"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C6:C16"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="B17:B26"/>
+    <mergeCell ref="C27:C36"/>
     <mergeCell ref="B6:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upd 30 apr v2
</commit_message>
<xml_diff>
--- a/useful/time_sheet.xlsx
+++ b/useful/time_sheet.xlsx
@@ -706,24 +706,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -737,6 +719,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1054,7 +1054,10 @@
   <dimension ref="A1:HT101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1082,32 +1085,32 @@
       <c r="I1" s="72"/>
       <c r="J1" s="23"/>
       <c r="K1" s="24"/>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
       <c r="Q1" s="20"/>
       <c r="R1" s="25"/>
-      <c r="S1" s="66" t="s">
+      <c r="S1" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
       <c r="X1" s="20"/>
       <c r="Y1" s="26"/>
-      <c r="Z1" s="66" t="s">
+      <c r="Z1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="67"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="61"/>
       <c r="AF1" s="21"/>
       <c r="AG1" s="21"/>
       <c r="AH1" s="22"/>
@@ -1831,7 +1834,7 @@
       </c>
       <c r="F4" s="42">
         <f t="shared" ref="F4:BQ4" si="0">SUM(F6:F101)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="47">
         <f t="shared" si="0"/>
@@ -1847,7 +1850,7 @@
       </c>
       <c r="J4" s="48">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K4" s="49">
         <f t="shared" si="0"/>
@@ -3400,10 +3403,10 @@
       </c>
     </row>
     <row r="6" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="60" t="s">
+      <c r="B6" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="52">
@@ -3490,8 +3493,8 @@
       <c r="HS6" s="7"/>
     </row>
     <row r="7" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="64"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="52">
         <v>1.2</v>
       </c>
@@ -3578,8 +3581,8 @@
       <c r="HS7" s="7"/>
     </row>
     <row r="8" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="64"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="52">
         <v>1.3</v>
       </c>
@@ -3664,8 +3667,8 @@
       <c r="HS8" s="7"/>
     </row>
     <row r="9" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="64"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="38">
         <v>1.4</v>
       </c>
@@ -3749,8 +3752,8 @@
       <c r="HS9" s="7"/>
     </row>
     <row r="10" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="64"/>
-      <c r="C10" s="60"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="38">
         <v>1.5</v>
       </c>
@@ -3832,8 +3835,8 @@
       <c r="HS10" s="7"/>
     </row>
     <row r="11" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="64"/>
-      <c r="C11" s="60"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="57">
         <v>1.6</v>
       </c>
@@ -3917,8 +3920,8 @@
       <c r="HS11" s="7"/>
     </row>
     <row r="12" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="64"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="38">
         <v>1.7</v>
       </c>
@@ -4000,8 +4003,8 @@
       <c r="HS12" s="7"/>
     </row>
     <row r="13" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="64"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="52">
         <v>1.8</v>
       </c>
@@ -4086,8 +4089,8 @@
       <c r="HS13" s="7"/>
     </row>
     <row r="14" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="64"/>
-      <c r="C14" s="60"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="57">
         <v>1.9</v>
       </c>
@@ -4171,8 +4174,8 @@
       <c r="HS14" s="7"/>
     </row>
     <row r="15" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="64"/>
-      <c r="C15" s="60"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="58">
         <v>1.1000000000000001</v>
       </c>
@@ -4256,8 +4259,8 @@
       <c r="HS15" s="7"/>
     </row>
     <row r="16" spans="1:228" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="65"/>
-      <c r="C16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="37"/>
       <c r="E16" s="14" t="s">
         <v>44</v>
@@ -4337,10 +4340,10 @@
       <c r="HS16" s="7"/>
     </row>
     <row r="17" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="65" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="53">
@@ -4426,8 +4429,8 @@
       <c r="HS17" s="7"/>
     </row>
     <row r="18" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="64"/>
-      <c r="C18" s="60"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="38">
         <v>2.2000000000000002</v>
       </c>
@@ -4509,8 +4512,8 @@
       <c r="HS18" s="7"/>
     </row>
     <row r="19" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="64"/>
-      <c r="C19" s="60"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="38">
         <v>2.2999999999999998</v>
       </c>
@@ -4592,8 +4595,8 @@
       <c r="HS19" s="7"/>
     </row>
     <row r="20" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="64"/>
-      <c r="C20" s="60"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="52">
         <v>2.4</v>
       </c>
@@ -4677,8 +4680,8 @@
       <c r="HS20" s="7"/>
     </row>
     <row r="21" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="64"/>
-      <c r="C21" s="60"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="38">
         <v>2.5</v>
       </c>
@@ -4762,18 +4765,22 @@
       <c r="HS21" s="7"/>
     </row>
     <row r="22" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="64"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="38">
+      <c r="B22" s="69"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="52">
         <v>2.6</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="F22" s="45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="J22" s="7">
+        <v>1</v>
+      </c>
       <c r="L22" s="9"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
@@ -4843,8 +4850,8 @@
       <c r="HS22" s="7"/>
     </row>
     <row r="23" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="64"/>
-      <c r="C23" s="60"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="38">
         <v>2.7</v>
       </c>
@@ -4924,8 +4931,8 @@
       <c r="HS23" s="7"/>
     </row>
     <row r="24" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="64"/>
-      <c r="C24" s="60"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="38">
         <v>2.8</v>
       </c>
@@ -5005,8 +5012,8 @@
       <c r="HS24" s="7"/>
     </row>
     <row r="25" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="64"/>
-      <c r="C25" s="60"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="38">
         <v>2.9</v>
       </c>
@@ -5086,8 +5093,8 @@
       <c r="HS25" s="7"/>
     </row>
     <row r="26" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="65"/>
-      <c r="C26" s="61"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="37"/>
       <c r="E26" s="14" t="s">
         <v>44</v>
@@ -5167,18 +5174,16 @@
       <c r="HS26" s="7"/>
     </row>
     <row r="27" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="62" t="s">
+      <c r="C27" s="65" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="39">
         <v>3.1</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="E27" s="11"/>
       <c r="F27" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5254,8 +5259,8 @@
       <c r="HS27" s="7"/>
     </row>
     <row r="28" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="64"/>
-      <c r="C28" s="60"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="38">
         <v>3.2</v>
       </c>
@@ -5337,8 +5342,8 @@
       <c r="HS28" s="7"/>
     </row>
     <row r="29" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="64"/>
-      <c r="C29" s="60"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="38">
         <v>3.3</v>
       </c>
@@ -5420,8 +5425,8 @@
       <c r="HS29" s="7"/>
     </row>
     <row r="30" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="64"/>
-      <c r="C30" s="60"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="38">
         <v>3.4</v>
       </c>
@@ -5503,8 +5508,8 @@
       <c r="HS30" s="7"/>
     </row>
     <row r="31" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="64"/>
-      <c r="C31" s="60"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="66"/>
       <c r="D31" s="38">
         <v>3.5</v>
       </c>
@@ -5586,8 +5591,8 @@
       <c r="HS31" s="7"/>
     </row>
     <row r="32" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="64"/>
-      <c r="C32" s="60"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="38">
         <v>3.6</v>
       </c>
@@ -5669,8 +5674,8 @@
       <c r="HS32" s="7"/>
     </row>
     <row r="33" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="64"/>
-      <c r="C33" s="60"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="66"/>
       <c r="D33" s="38">
         <v>3.7</v>
       </c>
@@ -5752,8 +5757,8 @@
       <c r="HS33" s="7"/>
     </row>
     <row r="34" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="64"/>
-      <c r="C34" s="60"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="66"/>
       <c r="D34" s="38">
         <v>3.8</v>
       </c>
@@ -5835,8 +5840,8 @@
       <c r="HS34" s="7"/>
     </row>
     <row r="35" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="64"/>
-      <c r="C35" s="60"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="38">
         <v>3.9</v>
       </c>
@@ -5916,8 +5921,8 @@
       <c r="HS35" s="7"/>
     </row>
     <row r="36" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="65"/>
-      <c r="C36" s="61"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="67"/>
       <c r="D36" s="37"/>
       <c r="E36" s="14" t="s">
         <v>44</v>
@@ -5997,10 +6002,10 @@
       <c r="HS36" s="7"/>
     </row>
     <row r="37" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="65" t="s">
         <v>21</v>
       </c>
       <c r="D37" s="39">
@@ -6084,8 +6089,8 @@
       <c r="HS37" s="7"/>
     </row>
     <row r="38" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="64"/>
-      <c r="C38" s="60"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="66"/>
       <c r="D38" s="38">
         <v>4.2</v>
       </c>
@@ -6167,8 +6172,8 @@
       <c r="HS38" s="7"/>
     </row>
     <row r="39" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="64"/>
-      <c r="C39" s="60"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="66"/>
       <c r="D39" s="38">
         <v>4.3</v>
       </c>
@@ -6250,8 +6255,8 @@
       <c r="HS39" s="7"/>
     </row>
     <row r="40" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="64"/>
-      <c r="C40" s="60"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="66"/>
       <c r="D40" s="38">
         <v>4.4000000000000004</v>
       </c>
@@ -6333,8 +6338,8 @@
       <c r="HS40" s="7"/>
     </row>
     <row r="41" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="64"/>
-      <c r="C41" s="60"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="66"/>
       <c r="D41" s="38">
         <v>4.5</v>
       </c>
@@ -6416,8 +6421,8 @@
       <c r="HS41" s="7"/>
     </row>
     <row r="42" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="60"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="66"/>
       <c r="D42" s="38">
         <v>4.5999999999999996</v>
       </c>
@@ -6499,8 +6504,8 @@
       <c r="HS42" s="7"/>
     </row>
     <row r="43" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="64"/>
-      <c r="C43" s="60"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="66"/>
       <c r="D43" s="38">
         <v>4.7</v>
       </c>
@@ -6582,8 +6587,8 @@
       <c r="HS43" s="7"/>
     </row>
     <row r="44" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="64"/>
-      <c r="C44" s="60"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="38">
         <v>4.8</v>
       </c>
@@ -6665,8 +6670,8 @@
       <c r="HS44" s="7"/>
     </row>
     <row r="45" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="64"/>
-      <c r="C45" s="60"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="66"/>
       <c r="D45" s="38">
         <v>4.9000000000000004</v>
       </c>
@@ -6746,8 +6751,8 @@
       <c r="HS45" s="7"/>
     </row>
     <row r="46" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="64"/>
-      <c r="C46" s="60"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="66"/>
       <c r="D46" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -6827,8 +6832,8 @@
       <c r="HS46" s="7"/>
     </row>
     <row r="47" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="65"/>
-      <c r="C47" s="61"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="67"/>
       <c r="D47" s="37"/>
       <c r="E47" s="14" t="s">
         <v>44</v>
@@ -6908,13 +6913,13 @@
       <c r="HS47" s="7"/>
     </row>
     <row r="48" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="62" t="s">
+      <c r="C48" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="39">
+      <c r="D48" s="53">
         <v>5.0999999999999996</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -6995,9 +7000,9 @@
       <c r="HS48" s="7"/>
     </row>
     <row r="49" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="64"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="38">
+      <c r="B49" s="69"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="52">
         <v>5.2</v>
       </c>
       <c r="E49" s="12" t="s">
@@ -7078,9 +7083,9 @@
       <c r="HS49" s="7"/>
     </row>
     <row r="50" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="64"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="38">
+      <c r="B50" s="69"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="52">
         <v>5.3</v>
       </c>
       <c r="E50" s="12" t="s">
@@ -7161,9 +7166,9 @@
       <c r="HS50" s="7"/>
     </row>
     <row r="51" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="64"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="38">
+      <c r="B51" s="69"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="52">
         <v>5.4</v>
       </c>
       <c r="E51" s="12" t="s">
@@ -7244,9 +7249,9 @@
       <c r="HS51" s="7"/>
     </row>
     <row r="52" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="64"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="38">
+      <c r="B52" s="69"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="52">
         <v>5.5</v>
       </c>
       <c r="E52" s="12" t="s">
@@ -7327,9 +7332,9 @@
       <c r="HS52" s="7"/>
     </row>
     <row r="53" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="64"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="38">
+      <c r="B53" s="69"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="52">
         <v>5.6</v>
       </c>
       <c r="E53" s="12" t="s">
@@ -7410,9 +7415,9 @@
       <c r="HS53" s="7"/>
     </row>
     <row r="54" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="64"/>
-      <c r="C54" s="60"/>
-      <c r="D54" s="38">
+      <c r="B54" s="69"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="52">
         <v>5.7</v>
       </c>
       <c r="E54" s="12" t="s">
@@ -7493,8 +7498,8 @@
       <c r="HS54" s="7"/>
     </row>
     <row r="55" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="64"/>
-      <c r="C55" s="60"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="66"/>
       <c r="D55" s="38">
         <v>5.8</v>
       </c>
@@ -7574,8 +7579,8 @@
       <c r="HS55" s="7"/>
     </row>
     <row r="56" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="64"/>
-      <c r="C56" s="60"/>
+      <c r="B56" s="69"/>
+      <c r="C56" s="66"/>
       <c r="D56" s="38">
         <v>5.9</v>
       </c>
@@ -7655,8 +7660,8 @@
       <c r="HS56" s="7"/>
     </row>
     <row r="57" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="65"/>
-      <c r="C57" s="61"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="67"/>
       <c r="D57" s="37"/>
       <c r="E57" s="14" t="s">
         <v>44</v>
@@ -7736,10 +7741,10 @@
       <c r="HS57" s="7"/>
     </row>
     <row r="58" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="63" t="s">
+      <c r="B58" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="62" t="s">
+      <c r="C58" s="65" t="s">
         <v>69</v>
       </c>
       <c r="D58" s="39">
@@ -7823,8 +7828,8 @@
       <c r="HS58" s="7"/>
     </row>
     <row r="59" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="64"/>
-      <c r="C59" s="60"/>
+      <c r="B59" s="69"/>
+      <c r="C59" s="66"/>
       <c r="D59" s="38">
         <v>6.2</v>
       </c>
@@ -7906,8 +7911,8 @@
       <c r="HS59" s="7"/>
     </row>
     <row r="60" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="64"/>
-      <c r="C60" s="60"/>
+      <c r="B60" s="69"/>
+      <c r="C60" s="66"/>
       <c r="D60" s="38">
         <v>6.3</v>
       </c>
@@ -7987,8 +7992,8 @@
       <c r="HS60" s="7"/>
     </row>
     <row r="61" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="64"/>
-      <c r="C61" s="60"/>
+      <c r="B61" s="69"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="38">
         <v>6.4</v>
       </c>
@@ -8068,8 +8073,8 @@
       <c r="HS61" s="7"/>
     </row>
     <row r="62" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="64"/>
-      <c r="C62" s="60"/>
+      <c r="B62" s="69"/>
+      <c r="C62" s="66"/>
       <c r="D62" s="38">
         <v>6.5</v>
       </c>
@@ -8149,8 +8154,8 @@
       <c r="HS62" s="7"/>
     </row>
     <row r="63" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B63" s="64"/>
-      <c r="C63" s="60"/>
+      <c r="B63" s="69"/>
+      <c r="C63" s="66"/>
       <c r="D63" s="38">
         <v>6.6</v>
       </c>
@@ -8230,8 +8235,8 @@
       <c r="HS63" s="7"/>
     </row>
     <row r="64" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="64"/>
-      <c r="C64" s="60"/>
+      <c r="B64" s="69"/>
+      <c r="C64" s="66"/>
       <c r="D64" s="38">
         <v>6.7</v>
       </c>
@@ -8311,8 +8316,8 @@
       <c r="HS64" s="7"/>
     </row>
     <row r="65" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="64"/>
-      <c r="C65" s="60"/>
+      <c r="B65" s="69"/>
+      <c r="C65" s="66"/>
       <c r="D65" s="38">
         <v>6.8</v>
       </c>
@@ -8392,8 +8397,8 @@
       <c r="HS65" s="7"/>
     </row>
     <row r="66" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="64"/>
-      <c r="C66" s="60"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="66"/>
       <c r="D66" s="38">
         <v>6.9</v>
       </c>
@@ -8473,8 +8478,8 @@
       <c r="HS66" s="7"/>
     </row>
     <row r="67" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="65"/>
-      <c r="C67" s="61"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="67"/>
       <c r="D67" s="37"/>
       <c r="E67" s="14" t="s">
         <v>44</v>
@@ -8554,10 +8559,10 @@
       <c r="HS67" s="7"/>
     </row>
     <row r="68" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="63" t="s">
+      <c r="B68" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C68" s="62" t="s">
+      <c r="C68" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D68" s="39">
@@ -8641,8 +8646,8 @@
       <c r="HS68" s="7"/>
     </row>
     <row r="69" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="64"/>
-      <c r="C69" s="60"/>
+      <c r="B69" s="69"/>
+      <c r="C69" s="66"/>
       <c r="D69" s="38">
         <v>7.2</v>
       </c>
@@ -8724,8 +8729,8 @@
       <c r="HS69" s="7"/>
     </row>
     <row r="70" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="64"/>
-      <c r="C70" s="60"/>
+      <c r="B70" s="69"/>
+      <c r="C70" s="66"/>
       <c r="D70" s="38">
         <v>7.3</v>
       </c>
@@ -8807,8 +8812,8 @@
       <c r="HS70" s="7"/>
     </row>
     <row r="71" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="64"/>
-      <c r="C71" s="60"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="66"/>
       <c r="D71" s="38">
         <v>7.4</v>
       </c>
@@ -8890,8 +8895,8 @@
       <c r="HS71" s="7"/>
     </row>
     <row r="72" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="64"/>
-      <c r="C72" s="60"/>
+      <c r="B72" s="69"/>
+      <c r="C72" s="66"/>
       <c r="D72" s="38">
         <v>7.5</v>
       </c>
@@ -8973,8 +8978,8 @@
       <c r="HS72" s="7"/>
     </row>
     <row r="73" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="60"/>
+      <c r="B73" s="69"/>
+      <c r="C73" s="66"/>
       <c r="D73" s="38">
         <v>7.6</v>
       </c>
@@ -9054,8 +9059,8 @@
       <c r="HS73" s="7"/>
     </row>
     <row r="74" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B74" s="64"/>
-      <c r="C74" s="60"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="66"/>
       <c r="D74" s="38">
         <v>7.7</v>
       </c>
@@ -9135,8 +9140,8 @@
       <c r="HS74" s="7"/>
     </row>
     <row r="75" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="64"/>
-      <c r="C75" s="60"/>
+      <c r="B75" s="69"/>
+      <c r="C75" s="66"/>
       <c r="D75" s="38">
         <v>7.8</v>
       </c>
@@ -9216,8 +9221,8 @@
       <c r="HS75" s="7"/>
     </row>
     <row r="76" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B76" s="64"/>
-      <c r="C76" s="60"/>
+      <c r="B76" s="69"/>
+      <c r="C76" s="66"/>
       <c r="D76" s="38">
         <v>7.9</v>
       </c>
@@ -9297,8 +9302,8 @@
       <c r="HS76" s="7"/>
     </row>
     <row r="77" spans="2:227" ht="15" x14ac:dyDescent="0.25">
-      <c r="B77" s="65"/>
-      <c r="C77" s="61"/>
+      <c r="B77" s="70"/>
+      <c r="C77" s="67"/>
       <c r="D77" s="37"/>
       <c r="E77" s="14" t="s">
         <v>44</v>
@@ -9378,10 +9383,10 @@
       <c r="HS77" s="7"/>
     </row>
     <row r="78" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="68" t="s">
+      <c r="B78" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="62" t="s">
+      <c r="C78" s="65" t="s">
         <v>55</v>
       </c>
       <c r="D78" s="39">
@@ -9463,8 +9468,8 @@
       <c r="HS78" s="7"/>
     </row>
     <row r="79" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="69"/>
-      <c r="C79" s="60"/>
+      <c r="B79" s="63"/>
+      <c r="C79" s="66"/>
       <c r="D79" s="38">
         <v>7.2</v>
       </c>
@@ -9544,8 +9549,8 @@
       <c r="HS79" s="7"/>
     </row>
     <row r="80" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="69"/>
-      <c r="C80" s="60"/>
+      <c r="B80" s="63"/>
+      <c r="C80" s="66"/>
       <c r="D80" s="38">
         <v>7.3</v>
       </c>
@@ -9625,8 +9630,8 @@
       <c r="HS80" s="7"/>
     </row>
     <row r="81" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="69"/>
-      <c r="C81" s="60"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="66"/>
       <c r="D81" s="38">
         <v>7.4</v>
       </c>
@@ -9706,8 +9711,8 @@
       <c r="HS81" s="7"/>
     </row>
     <row r="82" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="69"/>
-      <c r="C82" s="60"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="66"/>
       <c r="D82" s="38">
         <v>7.5</v>
       </c>
@@ -9787,8 +9792,8 @@
       <c r="HS82" s="7"/>
     </row>
     <row r="83" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="69"/>
-      <c r="C83" s="60"/>
+      <c r="B83" s="63"/>
+      <c r="C83" s="66"/>
       <c r="D83" s="38">
         <v>7.6</v>
       </c>
@@ -9868,8 +9873,8 @@
       <c r="HS83" s="7"/>
     </row>
     <row r="84" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="69"/>
-      <c r="C84" s="60"/>
+      <c r="B84" s="63"/>
+      <c r="C84" s="66"/>
       <c r="D84" s="38">
         <v>7.7</v>
       </c>
@@ -9949,8 +9954,8 @@
       <c r="HS84" s="7"/>
     </row>
     <row r="85" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="69"/>
-      <c r="C85" s="60"/>
+      <c r="B85" s="63"/>
+      <c r="C85" s="66"/>
       <c r="D85" s="38">
         <v>7.8</v>
       </c>
@@ -10030,8 +10035,8 @@
       <c r="HS85" s="7"/>
     </row>
     <row r="86" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="69"/>
-      <c r="C86" s="60"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="66"/>
       <c r="D86" s="38">
         <v>7.9</v>
       </c>
@@ -10111,8 +10116,8 @@
       <c r="HS86" s="7"/>
     </row>
     <row r="87" spans="2:227" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="70"/>
-      <c r="C87" s="61"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="67"/>
       <c r="D87" s="37"/>
       <c r="E87" s="14" t="s">
         <v>44</v>
@@ -11257,6 +11262,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C6:C16"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="B17:B26"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="B6:B16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="Z1:AE1"/>
     <mergeCell ref="S1:W1"/>
@@ -11273,12 +11284,6 @@
     <mergeCell ref="B37:B47"/>
     <mergeCell ref="B48:B57"/>
     <mergeCell ref="C48:C57"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C6:C16"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="B17:B26"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="B6:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>